<commit_message>
V1.5.5 Allow for subdomains
Subdomains allowed.  However 'www.'  is not allowed.  Potential domains starting with '.' will be ignored.
</commit_message>
<xml_diff>
--- a/excels_to_be_processed/dws_squid_test.xlsx
+++ b/excels_to_be_processed/dws_squid_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\anDREa_squid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\anDREa_squid\excels_to_be_processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B359E1B-5474-44B7-B995-1ECBC5B02150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D384E203-03A9-45C4-91C7-44E9B4B81754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35580" yWindow="2820" windowWidth="51060" windowHeight="15435" xr2:uid="{EB91D85B-3B10-4E01-B68C-94971D77060D}"/>
+    <workbookView xWindow="39585" yWindow="2985" windowWidth="14445" windowHeight="15435" xr2:uid="{EB91D85B-3B10-4E01-B68C-94971D77060D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="64">
   <si>
     <t>WorkspaceID</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>dws9900sayali</t>
+  </si>
+  <si>
+    <t>sub1.sub2.next.com</t>
   </si>
 </sst>
 </file>
@@ -624,13 +627,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA32C8D-AEDA-4870-A630-41EECB6AF2B4}">
-  <dimension ref="A1:FO22"/>
+  <dimension ref="A1:FP22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,12 +641,12 @@
     <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="2" customWidth="1"/>
-    <col min="4" max="65" width="4.42578125" style="2" customWidth="1"/>
-    <col min="66" max="171" width="9.140625" style="2"/>
-    <col min="172" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="66" width="4.42578125" style="2" customWidth="1"/>
+    <col min="67" max="172" width="9.140625" style="2"/>
+    <col min="173" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" s="4" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:84" s="4" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -669,38 +672,38 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="T1" s="4" t="s">
         <v>16</v>
       </c>
@@ -861,40 +864,43 @@
         <v>16</v>
       </c>
       <c r="BU1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="BV1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CF1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -913,9 +919,6 @@
       <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="J2" s="2" t="s">
         <v>1</v>
       </c>
@@ -928,7 +931,7 @@
       <c r="M2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="P2" s="2" t="s">
@@ -1135,8 +1138,11 @@
       <c r="CE2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1163,14 +1169,14 @@
       <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="BX4" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="O4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BY4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1183,11 +1189,11 @@
       <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="BZ5" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CA5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1209,8 +1215,11 @@
       <c r="K6" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="L6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1218,7 +1227,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -1226,7 +1235,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -1234,7 +1243,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1243,7 +1252,7 @@
       </c>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -1251,7 +1260,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -1259,7 +1268,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1267,7 +1276,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -1275,7 +1284,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -1283,7 +1292,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1342,9 +1351,9 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J1" r:id="rId1" xr:uid="{AD880A28-C4C8-48FC-9585-F5A45E28E3E5}"/>
-    <hyperlink ref="L1" r:id="rId2" xr:uid="{98FCB6ED-CCFA-41F5-8BF4-154FA2F8665B}"/>
-    <hyperlink ref="M1" r:id="rId3" xr:uid="{564EFEBE-2859-4B4F-AE83-7D3F82F116E1}"/>
+    <hyperlink ref="K1" r:id="rId1" xr:uid="{AD880A28-C4C8-48FC-9585-F5A45E28E3E5}"/>
+    <hyperlink ref="M1" r:id="rId2" xr:uid="{98FCB6ED-CCFA-41F5-8BF4-154FA2F8665B}"/>
+    <hyperlink ref="N1" r:id="rId3" xr:uid="{564EFEBE-2859-4B4F-AE83-7D3F82F116E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>